<commit_message>
after logout test done
</commit_message>
<xml_diff>
--- a/src/com/ptl/data/TestData.xlsx
+++ b/src/com/ptl/data/TestData.xlsx
@@ -4,20 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="19320" windowHeight="6420" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14715" windowHeight="3630" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Login Test" sheetId="2" r:id="rId2"/>
     <sheet name="Allocate Location Test" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:R20"/>
+  <oleSize ref="A1:M10"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>TCID</t>
   </si>
@@ -56,6 +59,24 @@
   </si>
   <si>
     <t>ward1</t>
+  </si>
+  <si>
+    <t>admin_welikada</t>
+  </si>
+  <si>
+    <t>test$123</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> test$123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test$123 </t>
+  </si>
+  <si>
+    <t>TEST$123</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -133,8 +154,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -485,10 +534,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="A1:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,7 +564,51 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -527,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
completed post registration authorize pages
</commit_message>
<xml_diff>
--- a/src/com/ptl/data/TestData.xlsx
+++ b/src/com/ptl/data/TestData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14715" windowHeight="6420" tabRatio="827" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14715" windowHeight="6420" tabRatio="827" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -13,17 +13,17 @@
     <sheet name="Inmate Registration-Personal" sheetId="7" r:id="rId4"/>
     <sheet name="Inmate Reg-Classification" sheetId="9" r:id="rId5"/>
     <sheet name="Inmate Reg-Characteristic" sheetId="10" r:id="rId6"/>
+    <sheet name="UpdatePostReg Test" sheetId="11" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="84">
   <si>
     <t>TCID</t>
   </si>
@@ -224,6 +224,57 @@
   </si>
   <si>
     <t>PassportNumber</t>
+  </si>
+  <si>
+    <t>Institues</t>
+  </si>
+  <si>
+    <t>Qualification Types</t>
+  </si>
+  <si>
+    <t>Languages</t>
+  </si>
+  <si>
+    <t>Employers</t>
+  </si>
+  <si>
+    <t>Organizational Types</t>
+  </si>
+  <si>
+    <t>Positions</t>
+  </si>
+  <si>
+    <t>Dates From</t>
+  </si>
+  <si>
+    <t>Dates To</t>
+  </si>
+  <si>
+    <t>Sri Lanka Insurance,Hatel Janaki</t>
+  </si>
+  <si>
+    <t>Private,Private</t>
+  </si>
+  <si>
+    <t>Trainee,Executive</t>
+  </si>
+  <si>
+    <t>2010-12-02,2013-12-02</t>
+  </si>
+  <si>
+    <t>2013-12-01,2015-01-02</t>
+  </si>
+  <si>
+    <t>UpdatePostReg Test</t>
+  </si>
+  <si>
+    <t>Piliyandala Central,Nalanda</t>
+  </si>
+  <si>
+    <t>Ordinary Level,Advance Level</t>
+  </si>
+  <si>
+    <t>Sinhala,English</t>
   </si>
 </sst>
 </file>
@@ -239,7 +290,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -249,6 +300,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -291,7 +348,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -299,6 +356,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,13 +700,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
     </row>
@@ -681,18 +740,29 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="7" t="s">
         <v>4</v>
       </c>
     </row>
@@ -980,7 +1050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
@@ -1055,4 +1125,87 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>